<commit_message>
2025-6-1 reset for HIRG anatomy WG
Selected the files needed for HIRG anatomy harmonization working group
</commit_message>
<xml_diff>
--- a/maps/anatomy/ICF-ICD-anatomy-v1.xlsx
+++ b/maps/anatomy/ICF-ICD-anatomy-v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tu/workspace/harmonization/maps/anatomy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1D143CFF-46F4-A848-9FF9-743F6E447EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC32F436-5331-E74C-A0C2-09C85CE22165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9540" yWindow="11120" windowWidth="27240" windowHeight="16440"/>
+    <workbookView xWindow="18660" yWindow="1820" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ICF-ICD-anatomy-v1 copy" sheetId="1" r:id="rId1"/>
@@ -1579,7 +1579,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2434,19 +2434,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F418"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A366" workbookViewId="0">
-      <selection activeCell="A366" sqref="A1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A376" workbookViewId="0">
+      <selection activeCell="A376" sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" style="1" customWidth="1"/>
-    <col min="4" max="6" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="39.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>